<commit_message>
method to create & update woo
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aldyhameshastudio\Projects\woo-products-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E506EA-3771-4C20-9B59-A8C5E50591A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC7C29A-B208-45E4-842D-F914928172AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC029AD2-2B72-4F45-9D44-4605493134C9}"/>
   </bookViews>
@@ -36,57 +36,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>SKU</t>
   </si>
   <si>
-    <t>Produk 1</t>
-  </si>
-  <si>
-    <t>Produk 2</t>
-  </si>
-  <si>
-    <t>A01</t>
-  </si>
-  <si>
-    <t>A02</t>
-  </si>
-  <si>
-    <t>A03</t>
-  </si>
-  <si>
-    <t>ini deskripsi</t>
-  </si>
-  <si>
-    <t>ini deskripsi 2</t>
-  </si>
-  <si>
-    <t>ini deskripsi 3</t>
-  </si>
-  <si>
-    <t>simple</t>
-  </si>
-  <si>
     <t>NAME</t>
   </si>
   <si>
     <t>PRICE</t>
   </si>
   <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>ID PRODUCT</t>
-  </si>
-  <si>
-    <t>ID PARENT</t>
-  </si>
-  <si>
-    <t>Produk 333</t>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>SUBCATEGORY</t>
+  </si>
+  <si>
+    <t>Furniture</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Kursi Santai</t>
+  </si>
+  <si>
+    <t>P01A</t>
+  </si>
+  <si>
+    <t>P01B</t>
+  </si>
+  <si>
+    <t>DIMENSION</t>
+  </si>
+  <si>
+    <t>AREA</t>
+  </si>
+  <si>
+    <t>100 x 100</t>
+  </si>
+  <si>
+    <t>INDOOR</t>
+  </si>
+  <si>
+    <t>OUTDOOR</t>
+  </si>
+  <si>
+    <t>Meja besar</t>
+  </si>
+  <si>
+    <t>P02A</t>
+  </si>
+  <si>
+    <t>100 x 200 x 300</t>
+  </si>
+  <si>
+    <t>P02B</t>
+  </si>
+  <si>
+    <t>P02C</t>
+  </si>
+  <si>
+    <t>P02E</t>
+  </si>
+  <si>
+    <t>200 x 200 x 300</t>
+  </si>
+  <si>
+    <t>200 x 200</t>
+  </si>
+  <si>
+    <t>Sofa</t>
+  </si>
+  <si>
+    <t>P03A</t>
+  </si>
+  <si>
+    <t>P03B</t>
   </si>
 </sst>
 </file>
@@ -453,101 +483,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7252D55-D232-408C-BCF5-DC7E567871F0}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="6" max="6" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E2">
-        <v>1000</v>
+        <v>9999</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>2000</v>
+        <v>39999</v>
       </c>
       <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>5000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="E4">
-        <v>3000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>6000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>7000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>8500</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>1000</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>2000</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>